<commit_message>
fixed col names in raw data
</commit_message>
<xml_diff>
--- a/data/USFWS_bull_trout_SSA_data_ID_HellsCanyon.xlsx
+++ b/data/USFWS_bull_trout_SSA_data_ID_HellsCanyon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DNolfi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E9573AF-B2BD-4C2D-BFF0-F66167DC5DE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8404F2-985D-0246-AFF9-A11876E6CCAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ID_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="23">
   <si>
     <t>recovery unit</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Both of these data sets are thought to cover mostly the Imnaha Core Area (75%) and the remaining 25% being split between Grand Ronde and Little Lower Salmon</t>
+  </si>
+  <si>
+    <t>dataset</t>
   </si>
 </sst>
 </file>
@@ -639,25 +642,25 @@
   <dimension ref="A1:BB1263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="15"/>
-    <col min="2" max="2" width="19.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="45.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="45.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.83203125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" style="15" customWidth="1"/>
     <col min="10" max="16384" width="11" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -693,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -773,7 +776,7 @@
       <c r="BA2" s="16"/>
       <c r="BB2" s="16"/>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -811,7 +814,7 @@
         <v>0.23098456393703048</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>1</v>
       </c>
@@ -849,7 +852,7 @@
         <v>0.10323382874284411</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <v>1</v>
       </c>
@@ -887,7 +890,7 @@
         <v>0.10542170028331849</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>1</v>
       </c>
@@ -925,7 +928,7 @@
         <v>7.3687964340974577E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <v>1</v>
       </c>
@@ -963,7 +966,7 @@
         <v>6.5353807976494788E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <v>1</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>7.3873016131666747E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <v>1</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>0.11583737532353203</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>1</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>0.10338019530836812</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>1</v>
       </c>
@@ -1115,7 +1118,7 @@
         <v>8.6527552465274854E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <v>1</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>8.3017593019200406E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <v>2</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>0.34679260093882802</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <v>2</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>0.15005052358339643</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <v>2</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>0.15805824678521008</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <v>2</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>0.16436680582592952</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
         <v>2</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>0.15972779618484284</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
         <v>2</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>0.14048150895563999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
         <v>2</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>0.14629047168935819</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
         <v>2</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>0.12244057101284238</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
         <v>2</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>0.125583532270888</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
         <v>2</v>
       </c>
@@ -1533,3113 +1536,3113 @@
         <v>0.12643866342754281</v>
       </c>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H61" s="17"/>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H62" s="17"/>
     </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H63" s="17"/>
     </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H64" s="17"/>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H65" s="17"/>
     </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H66" s="17"/>
     </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H67" s="17"/>
     </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H68" s="17"/>
     </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H69" s="17"/>
     </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H70" s="17"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H71" s="17"/>
     </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H72" s="17"/>
     </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H73" s="17"/>
     </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H74" s="17"/>
     </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H75" s="17"/>
     </row>
-    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H76" s="17"/>
     </row>
-    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H77" s="17"/>
     </row>
-    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H78" s="17"/>
     </row>
-    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H79" s="17"/>
     </row>
-    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H80" s="17"/>
     </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H81" s="17"/>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H82" s="17"/>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H83" s="17"/>
     </row>
-    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H84" s="17"/>
     </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H85" s="17"/>
     </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H86" s="17"/>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H87" s="17"/>
     </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H88" s="17"/>
     </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H89" s="17"/>
     </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H90" s="17"/>
     </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H91" s="17"/>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H92" s="17"/>
     </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H93" s="17"/>
     </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H94" s="17"/>
     </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H95" s="17"/>
     </row>
-    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H146" s="17"/>
     </row>
-    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H147" s="17"/>
     </row>
-    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H148" s="17"/>
     </row>
-    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H149" s="17"/>
     </row>
-    <row r="150" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H150" s="17"/>
     </row>
-    <row r="151" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H151" s="17"/>
     </row>
-    <row r="152" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H152" s="17"/>
     </row>
-    <row r="153" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H153" s="17"/>
     </row>
-    <row r="154" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H154" s="17"/>
     </row>
-    <row r="155" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H155" s="17"/>
     </row>
-    <row r="156" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H156" s="17"/>
     </row>
-    <row r="157" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H157" s="17"/>
     </row>
-    <row r="158" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H158" s="17"/>
     </row>
-    <row r="159" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H159" s="17"/>
     </row>
-    <row r="160" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H160" s="17"/>
     </row>
-    <row r="161" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H161" s="17"/>
     </row>
-    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H162" s="17"/>
     </row>
-    <row r="163" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H163" s="17"/>
     </row>
-    <row r="164" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H164" s="17"/>
     </row>
-    <row r="165" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H165" s="17"/>
     </row>
-    <row r="166" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H166" s="17"/>
     </row>
-    <row r="167" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H167" s="17"/>
     </row>
-    <row r="168" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H168" s="17"/>
     </row>
-    <row r="169" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H169" s="17"/>
     </row>
-    <row r="170" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H170" s="17"/>
     </row>
-    <row r="171" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H171" s="17"/>
     </row>
-    <row r="172" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H172" s="17"/>
     </row>
-    <row r="173" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H173" s="17"/>
     </row>
-    <row r="207" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H207" s="17"/>
     </row>
-    <row r="208" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H208" s="17"/>
     </row>
-    <row r="209" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H209" s="17"/>
     </row>
-    <row r="210" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H210" s="17"/>
     </row>
-    <row r="211" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H211" s="17"/>
     </row>
-    <row r="212" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H212" s="17"/>
     </row>
-    <row r="213" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H213" s="17"/>
     </row>
-    <row r="214" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H214" s="17"/>
     </row>
-    <row r="215" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H215" s="17"/>
     </row>
-    <row r="216" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H216" s="17"/>
     </row>
-    <row r="217" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H217" s="17"/>
     </row>
-    <row r="218" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H218" s="17"/>
     </row>
-    <row r="219" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H219" s="17"/>
     </row>
-    <row r="220" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H220" s="17"/>
     </row>
-    <row r="221" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H221" s="17"/>
     </row>
-    <row r="222" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H222" s="17"/>
     </row>
-    <row r="223" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H223" s="17"/>
     </row>
-    <row r="224" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H224" s="17"/>
     </row>
-    <row r="225" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H225" s="17"/>
     </row>
-    <row r="226" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H226" s="17"/>
     </row>
-    <row r="227" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H227" s="17"/>
     </row>
-    <row r="228" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H228" s="17"/>
     </row>
-    <row r="229" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H229" s="17"/>
     </row>
-    <row r="230" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H230" s="17"/>
     </row>
-    <row r="231" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H231" s="17"/>
     </row>
-    <row r="232" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H232" s="17"/>
     </row>
-    <row r="233" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H233" s="17"/>
     </row>
-    <row r="234" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H234" s="17"/>
     </row>
-    <row r="235" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H235" s="17"/>
     </row>
-    <row r="236" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H236" s="17"/>
     </row>
-    <row r="237" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H237" s="17"/>
     </row>
-    <row r="238" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H238" s="17"/>
     </row>
-    <row r="239" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H239" s="17"/>
     </row>
-    <row r="240" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H240" s="17"/>
     </row>
-    <row r="241" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H241" s="17"/>
     </row>
-    <row r="242" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H242" s="17"/>
     </row>
-    <row r="243" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H243" s="17"/>
     </row>
-    <row r="244" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H244" s="17"/>
     </row>
-    <row r="245" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H245" s="17"/>
     </row>
-    <row r="246" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H246" s="17"/>
     </row>
-    <row r="247" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H247" s="17"/>
     </row>
-    <row r="248" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H248" s="17"/>
     </row>
-    <row r="249" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H249" s="17"/>
     </row>
-    <row r="250" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H250" s="17"/>
     </row>
-    <row r="251" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H251" s="17"/>
     </row>
-    <row r="252" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H252" s="17"/>
     </row>
-    <row r="253" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H253" s="17"/>
     </row>
-    <row r="254" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H254" s="17"/>
     </row>
-    <row r="255" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H255" s="17"/>
     </row>
-    <row r="256" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H256" s="17"/>
     </row>
-    <row r="257" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H257" s="17"/>
     </row>
-    <row r="258" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H258" s="17"/>
     </row>
-    <row r="259" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H259" s="17"/>
     </row>
-    <row r="260" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H260" s="17"/>
     </row>
-    <row r="261" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H261" s="17"/>
     </row>
-    <row r="262" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H262" s="17"/>
     </row>
-    <row r="263" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H263" s="17"/>
     </row>
-    <row r="264" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H264" s="17"/>
     </row>
-    <row r="265" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H265" s="17"/>
     </row>
-    <row r="266" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H266" s="17"/>
     </row>
-    <row r="267" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H267" s="17"/>
     </row>
-    <row r="268" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H268" s="17"/>
     </row>
-    <row r="269" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H269" s="17"/>
     </row>
-    <row r="270" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H270" s="17"/>
     </row>
-    <row r="271" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H271" s="17"/>
     </row>
-    <row r="272" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H272" s="17"/>
     </row>
-    <row r="273" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H273" s="17"/>
     </row>
-    <row r="274" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H274" s="17"/>
     </row>
-    <row r="275" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H275" s="17"/>
     </row>
-    <row r="276" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H276" s="17"/>
     </row>
-    <row r="277" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H277" s="17"/>
     </row>
-    <row r="278" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H278" s="17"/>
     </row>
-    <row r="279" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H279" s="17"/>
     </row>
-    <row r="280" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H280" s="17"/>
     </row>
-    <row r="281" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H281" s="17"/>
     </row>
-    <row r="282" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H282" s="17"/>
     </row>
-    <row r="283" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H283" s="17"/>
     </row>
-    <row r="284" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H284" s="17"/>
     </row>
-    <row r="285" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H285" s="17"/>
     </row>
-    <row r="286" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H286" s="17"/>
     </row>
-    <row r="287" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H287" s="17"/>
     </row>
-    <row r="334" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H334" s="18"/>
     </row>
-    <row r="335" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H335" s="18"/>
     </row>
-    <row r="336" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H336" s="18"/>
     </row>
-    <row r="337" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H337" s="18"/>
     </row>
-    <row r="338" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H338" s="18"/>
     </row>
-    <row r="339" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H339" s="18"/>
     </row>
-    <row r="340" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H340" s="18"/>
     </row>
-    <row r="341" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H341" s="18"/>
     </row>
-    <row r="342" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H342" s="18"/>
     </row>
-    <row r="343" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H343" s="18"/>
     </row>
-    <row r="344" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H344" s="18"/>
     </row>
-    <row r="345" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H345" s="18"/>
     </row>
-    <row r="346" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H346" s="18"/>
     </row>
-    <row r="347" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H347" s="18"/>
     </row>
-    <row r="348" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H348" s="18"/>
     </row>
-    <row r="349" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H349" s="18"/>
     </row>
-    <row r="381" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H381" s="17"/>
     </row>
-    <row r="382" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H382" s="17"/>
     </row>
-    <row r="383" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H383" s="17"/>
     </row>
-    <row r="384" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H384" s="17"/>
     </row>
-    <row r="385" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H385" s="17"/>
     </row>
-    <row r="386" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H386" s="17"/>
     </row>
-    <row r="387" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H387" s="17"/>
     </row>
-    <row r="388" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H388" s="17"/>
     </row>
-    <row r="389" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H389" s="17"/>
     </row>
-    <row r="390" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H390" s="17"/>
     </row>
-    <row r="391" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H391" s="17"/>
     </row>
-    <row r="392" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H392" s="17"/>
     </row>
-    <row r="393" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H393" s="17"/>
     </row>
-    <row r="394" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H394" s="17"/>
     </row>
-    <row r="395" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H395" s="17"/>
     </row>
-    <row r="403" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H403" s="18"/>
     </row>
-    <row r="404" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H404" s="18"/>
     </row>
-    <row r="405" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H405" s="19"/>
     </row>
-    <row r="406" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H406" s="19"/>
     </row>
-    <row r="407" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H407" s="19"/>
     </row>
-    <row r="408" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H408" s="19"/>
     </row>
-    <row r="409" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H409" s="19"/>
     </row>
-    <row r="410" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H410" s="19"/>
     </row>
-    <row r="411" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H411" s="19"/>
     </row>
-    <row r="412" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H412" s="19"/>
     </row>
-    <row r="413" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H413" s="19"/>
     </row>
-    <row r="414" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H414" s="19"/>
     </row>
-    <row r="415" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H415" s="19"/>
     </row>
-    <row r="416" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="416" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H416" s="19"/>
     </row>
-    <row r="417" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="417" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H417" s="19"/>
     </row>
-    <row r="440" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="440" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H440" s="18"/>
     </row>
-    <row r="441" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="441" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H441" s="18"/>
     </row>
-    <row r="442" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="442" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H442" s="18"/>
     </row>
-    <row r="443" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="443" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H443" s="18"/>
     </row>
-    <row r="444" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="444" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H444" s="18"/>
     </row>
-    <row r="445" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="445" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H445" s="18"/>
     </row>
-    <row r="446" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="446" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H446" s="18"/>
     </row>
-    <row r="447" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="447" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H447" s="18"/>
     </row>
-    <row r="448" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="448" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H448" s="18"/>
     </row>
-    <row r="456" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="456" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H456" s="18"/>
     </row>
-    <row r="457" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="457" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H457" s="17"/>
     </row>
-    <row r="458" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="458" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H458" s="17"/>
     </row>
-    <row r="459" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="459" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H459" s="17"/>
     </row>
-    <row r="460" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="460" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H460" s="17"/>
     </row>
-    <row r="461" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="461" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H461" s="17"/>
     </row>
-    <row r="462" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="462" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H462" s="17"/>
     </row>
-    <row r="463" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="463" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H463" s="17"/>
     </row>
-    <row r="464" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="464" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H464" s="17"/>
     </row>
-    <row r="465" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="465" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H465" s="17"/>
     </row>
-    <row r="466" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="466" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H466" s="17"/>
     </row>
-    <row r="467" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="467" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H467" s="17"/>
     </row>
-    <row r="468" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="468" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H468" s="17"/>
     </row>
-    <row r="469" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="469" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H469" s="17"/>
     </row>
-    <row r="470" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="470" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H470" s="17"/>
     </row>
-    <row r="479" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="479" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H479" s="17"/>
     </row>
-    <row r="480" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="480" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H480" s="17"/>
     </row>
-    <row r="481" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="481" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H481" s="17"/>
     </row>
-    <row r="482" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="482" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H482" s="17"/>
     </row>
-    <row r="483" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="483" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H483" s="17"/>
     </row>
-    <row r="484" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="484" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H484" s="17"/>
     </row>
-    <row r="485" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="485" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H485" s="17"/>
     </row>
-    <row r="486" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="486" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H486" s="17"/>
     </row>
-    <row r="487" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="487" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H487" s="17"/>
     </row>
-    <row r="488" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="488" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H488" s="17"/>
     </row>
-    <row r="489" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="489" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H489" s="17"/>
     </row>
-    <row r="490" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="490" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H490" s="17"/>
     </row>
-    <row r="491" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="491" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H491" s="17"/>
     </row>
-    <row r="492" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="492" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H492" s="17"/>
     </row>
-    <row r="493" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="493" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H493" s="17"/>
     </row>
-    <row r="494" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="494" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H494" s="17"/>
     </row>
-    <row r="495" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="495" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H495" s="17"/>
     </row>
-    <row r="496" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="496" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H496" s="17"/>
     </row>
-    <row r="497" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="497" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H497" s="17"/>
     </row>
-    <row r="498" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="498" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H498" s="17"/>
     </row>
-    <row r="499" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="499" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H499" s="17"/>
     </row>
-    <row r="500" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="500" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H500" s="17"/>
     </row>
-    <row r="501" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="501" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H501" s="17"/>
     </row>
-    <row r="502" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="502" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H502" s="17"/>
     </row>
-    <row r="503" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="503" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H503" s="17"/>
     </row>
-    <row r="504" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="504" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G504" s="13"/>
       <c r="H504" s="13"/>
     </row>
-    <row r="505" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="505" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G505" s="13"/>
       <c r="H505" s="13"/>
     </row>
-    <row r="506" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="506" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G506" s="13"/>
       <c r="H506" s="13"/>
     </row>
-    <row r="507" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="507" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G507" s="13"/>
       <c r="H507" s="13"/>
     </row>
-    <row r="508" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="508" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G508" s="13"/>
       <c r="H508" s="13"/>
     </row>
-    <row r="509" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="509" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G509" s="13"/>
       <c r="H509" s="13"/>
     </row>
-    <row r="510" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="510" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G510" s="13"/>
       <c r="H510" s="13"/>
     </row>
-    <row r="511" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="511" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G511" s="13"/>
       <c r="H511" s="13"/>
     </row>
-    <row r="512" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="512" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G512" s="13"/>
       <c r="H512" s="13"/>
     </row>
-    <row r="513" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="513" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G513" s="13"/>
       <c r="H513" s="13"/>
     </row>
-    <row r="514" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="514" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G514" s="13"/>
       <c r="H514" s="13"/>
     </row>
-    <row r="515" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="515" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G515" s="13"/>
       <c r="H515" s="13"/>
     </row>
-    <row r="516" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="516" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G516" s="13"/>
       <c r="H516" s="13"/>
     </row>
-    <row r="517" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="517" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G517" s="13"/>
       <c r="H517" s="13"/>
     </row>
-    <row r="518" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="518" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G518" s="13"/>
       <c r="H518" s="13"/>
     </row>
-    <row r="519" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="519" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G519" s="13"/>
       <c r="H519" s="13"/>
     </row>
-    <row r="520" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="520" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G520" s="13"/>
       <c r="H520" s="13"/>
     </row>
-    <row r="521" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="521" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G521" s="13"/>
       <c r="H521" s="13"/>
     </row>
-    <row r="522" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="522" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G522" s="13"/>
       <c r="H522" s="13"/>
     </row>
-    <row r="523" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="523" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G523" s="13"/>
       <c r="H523" s="13"/>
     </row>
-    <row r="524" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="524" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G524" s="13"/>
       <c r="H524" s="13"/>
     </row>
-    <row r="525" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="525" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G525" s="13"/>
       <c r="H525" s="13"/>
     </row>
-    <row r="526" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="526" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G526" s="13"/>
       <c r="H526" s="13"/>
     </row>
-    <row r="527" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="527" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G527" s="13"/>
       <c r="H527" s="13"/>
     </row>
-    <row r="528" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="528" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G528" s="13"/>
       <c r="H528" s="13"/>
     </row>
-    <row r="529" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="529" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G529" s="13"/>
       <c r="H529" s="13"/>
     </row>
-    <row r="530" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="530" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G530" s="13"/>
       <c r="H530" s="13"/>
     </row>
-    <row r="531" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="531" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G531" s="13"/>
       <c r="H531" s="13"/>
     </row>
-    <row r="532" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="532" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G532" s="13"/>
       <c r="H532" s="13"/>
     </row>
-    <row r="533" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="533" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G533" s="13"/>
       <c r="H533" s="13"/>
     </row>
-    <row r="534" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="534" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G534" s="13"/>
       <c r="H534" s="13"/>
     </row>
-    <row r="535" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="535" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G535" s="13"/>
       <c r="H535" s="13"/>
     </row>
-    <row r="536" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="536" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G536" s="13"/>
       <c r="H536" s="13"/>
     </row>
-    <row r="537" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="537" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G537" s="13"/>
       <c r="H537" s="13"/>
     </row>
-    <row r="538" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="538" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G538" s="13"/>
       <c r="H538" s="13"/>
     </row>
-    <row r="539" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="539" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G539" s="13"/>
       <c r="H539" s="13"/>
     </row>
-    <row r="540" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="540" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G540" s="13"/>
       <c r="H540" s="13"/>
     </row>
-    <row r="541" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="541" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G541" s="13"/>
       <c r="H541" s="13"/>
     </row>
-    <row r="542" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="542" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G542" s="13"/>
       <c r="H542" s="13"/>
     </row>
-    <row r="543" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="543" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G543" s="13"/>
       <c r="H543" s="13"/>
     </row>
-    <row r="544" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="544" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G544" s="13"/>
       <c r="H544" s="13"/>
     </row>
-    <row r="545" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="545" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G545" s="13"/>
       <c r="H545" s="13"/>
     </row>
-    <row r="546" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="546" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G546" s="13"/>
       <c r="H546" s="13"/>
     </row>
-    <row r="547" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="547" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G547" s="13"/>
       <c r="H547" s="13"/>
     </row>
-    <row r="548" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="548" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G548" s="13"/>
       <c r="H548" s="13"/>
     </row>
-    <row r="549" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="549" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G549" s="13"/>
       <c r="H549" s="13"/>
     </row>
-    <row r="550" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="550" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G550" s="13"/>
       <c r="H550" s="13"/>
     </row>
-    <row r="551" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="551" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G551" s="13"/>
       <c r="H551" s="13"/>
     </row>
-    <row r="552" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="552" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G552" s="13"/>
       <c r="H552" s="13"/>
     </row>
-    <row r="553" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="553" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G553" s="13"/>
       <c r="H553" s="13"/>
     </row>
-    <row r="554" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="554" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G554" s="13"/>
       <c r="H554" s="13"/>
     </row>
-    <row r="555" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="555" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G555" s="13"/>
       <c r="H555" s="13"/>
     </row>
-    <row r="556" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="556" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G556" s="13"/>
       <c r="H556" s="13"/>
     </row>
-    <row r="557" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="557" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G557" s="13"/>
       <c r="H557" s="13"/>
     </row>
-    <row r="558" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="558" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G558" s="13"/>
       <c r="H558" s="13"/>
     </row>
-    <row r="559" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="559" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G559" s="13"/>
       <c r="H559" s="13"/>
     </row>
-    <row r="560" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="560" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G560" s="13"/>
       <c r="H560" s="13"/>
     </row>
-    <row r="561" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="561" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G561" s="13"/>
       <c r="H561" s="13"/>
     </row>
-    <row r="562" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="562" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G562" s="13"/>
       <c r="H562" s="13"/>
     </row>
-    <row r="563" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="563" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G563" s="13"/>
       <c r="H563" s="13"/>
     </row>
-    <row r="564" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="564" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G564" s="13"/>
       <c r="H564" s="13"/>
     </row>
-    <row r="565" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="565" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G565" s="13"/>
       <c r="H565" s="19"/>
     </row>
-    <row r="566" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="566" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G566" s="13"/>
       <c r="H566" s="13"/>
     </row>
-    <row r="567" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="567" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G567" s="13"/>
       <c r="H567" s="19"/>
     </row>
-    <row r="568" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="568" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G568" s="13"/>
       <c r="H568" s="19"/>
     </row>
-    <row r="569" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="569" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G569" s="13"/>
       <c r="H569" s="19"/>
     </row>
-    <row r="570" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="570" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G570" s="13"/>
       <c r="H570" s="19"/>
     </row>
-    <row r="571" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="571" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G571" s="13"/>
       <c r="H571" s="19"/>
     </row>
-    <row r="572" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="572" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G572" s="13"/>
       <c r="H572" s="19"/>
     </row>
-    <row r="573" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="573" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G573" s="13"/>
       <c r="H573" s="19"/>
     </row>
-    <row r="574" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="574" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G574" s="13"/>
       <c r="H574" s="19"/>
     </row>
-    <row r="575" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="575" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G575" s="13"/>
       <c r="H575" s="19"/>
     </row>
-    <row r="576" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="576" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G576" s="13"/>
       <c r="H576" s="19"/>
     </row>
-    <row r="577" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="577" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G577" s="13"/>
       <c r="H577" s="19"/>
     </row>
-    <row r="578" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="578" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G578" s="13"/>
       <c r="H578" s="19"/>
     </row>
-    <row r="579" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="579" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G579" s="13"/>
       <c r="H579" s="19"/>
     </row>
-    <row r="580" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="580" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G580" s="13"/>
       <c r="H580" s="19"/>
     </row>
-    <row r="581" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="581" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G581" s="13"/>
       <c r="H581" s="19"/>
     </row>
-    <row r="582" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="582" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G582" s="13"/>
       <c r="H582" s="19"/>
     </row>
-    <row r="583" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="583" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G583" s="13"/>
       <c r="H583" s="19"/>
     </row>
-    <row r="584" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="584" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G584" s="13"/>
       <c r="H584" s="19"/>
     </row>
-    <row r="585" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="585" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G585" s="13"/>
       <c r="H585" s="19"/>
     </row>
-    <row r="586" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="586" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G586" s="13"/>
       <c r="H586" s="19"/>
     </row>
-    <row r="587" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="587" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G587" s="13"/>
       <c r="H587" s="19"/>
     </row>
-    <row r="588" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="588" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G588" s="13"/>
       <c r="H588" s="19"/>
     </row>
-    <row r="589" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="589" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G589" s="13"/>
       <c r="H589" s="19"/>
     </row>
-    <row r="590" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="590" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G590" s="13"/>
       <c r="H590" s="19"/>
     </row>
-    <row r="591" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="591" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G591" s="13"/>
       <c r="H591" s="13"/>
     </row>
-    <row r="592" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="592" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G592" s="13"/>
       <c r="H592" s="13"/>
     </row>
-    <row r="593" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="593" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G593" s="13"/>
       <c r="H593" s="13"/>
     </row>
-    <row r="594" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="594" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G594" s="13"/>
       <c r="H594" s="13"/>
     </row>
-    <row r="595" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="595" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G595" s="13"/>
       <c r="H595" s="13"/>
     </row>
-    <row r="596" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="596" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G596" s="13"/>
       <c r="H596" s="13"/>
     </row>
-    <row r="597" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="597" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G597" s="13"/>
       <c r="H597" s="13"/>
     </row>
-    <row r="598" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="598" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G598" s="13"/>
       <c r="H598" s="13"/>
     </row>
-    <row r="599" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="599" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G599" s="13"/>
       <c r="H599" s="13"/>
     </row>
-    <row r="600" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="600" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G600" s="13"/>
       <c r="H600" s="13"/>
     </row>
-    <row r="601" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="601" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G601" s="13"/>
       <c r="H601" s="13"/>
     </row>
-    <row r="602" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="602" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G602" s="13"/>
       <c r="H602" s="13"/>
     </row>
-    <row r="603" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="603" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G603" s="13"/>
       <c r="H603" s="13"/>
     </row>
-    <row r="604" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="604" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G604" s="13"/>
       <c r="H604" s="13"/>
     </row>
-    <row r="605" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="605" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G605" s="13"/>
       <c r="H605" s="13"/>
     </row>
-    <row r="606" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="606" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G606" s="13"/>
       <c r="H606" s="13"/>
     </row>
-    <row r="607" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="607" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G607" s="13"/>
       <c r="H607" s="13"/>
     </row>
-    <row r="608" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="608" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G608" s="13"/>
       <c r="H608" s="13"/>
     </row>
-    <row r="609" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="609" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G609" s="13"/>
       <c r="H609" s="13"/>
     </row>
-    <row r="610" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="610" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G610" s="13"/>
       <c r="H610" s="13"/>
     </row>
-    <row r="611" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="611" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G611" s="13"/>
       <c r="H611" s="13"/>
     </row>
-    <row r="612" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="612" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G612" s="13"/>
       <c r="H612" s="13"/>
     </row>
-    <row r="613" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="613" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G613" s="13"/>
       <c r="H613" s="13"/>
     </row>
-    <row r="614" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="614" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G614" s="13"/>
       <c r="H614" s="13"/>
     </row>
-    <row r="615" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="615" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G615" s="13"/>
       <c r="H615" s="19"/>
     </row>
-    <row r="616" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="616" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G616" s="13"/>
       <c r="H616" s="13"/>
     </row>
-    <row r="617" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="617" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G617" s="13"/>
       <c r="H617" s="19"/>
     </row>
-    <row r="618" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="618" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G618" s="13"/>
       <c r="H618" s="19"/>
     </row>
-    <row r="619" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="619" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G619" s="13"/>
       <c r="H619" s="19"/>
     </row>
-    <row r="620" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="620" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G620" s="13"/>
       <c r="H620" s="19"/>
     </row>
-    <row r="621" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="621" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G621" s="13"/>
       <c r="H621" s="19"/>
     </row>
-    <row r="622" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="622" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G622" s="13"/>
       <c r="H622" s="19"/>
     </row>
-    <row r="623" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="623" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G623" s="13"/>
       <c r="H623" s="19"/>
     </row>
-    <row r="624" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="624" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G624" s="13"/>
       <c r="H624" s="19"/>
     </row>
-    <row r="625" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="625" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G625" s="13"/>
       <c r="H625" s="19"/>
     </row>
-    <row r="626" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="626" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G626" s="13"/>
       <c r="H626" s="19"/>
     </row>
-    <row r="627" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="627" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G627" s="13"/>
       <c r="H627" s="19"/>
     </row>
-    <row r="628" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="628" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G628" s="13"/>
       <c r="H628" s="13"/>
     </row>
-    <row r="629" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="629" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G629" s="13"/>
       <c r="H629" s="13"/>
     </row>
-    <row r="630" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="630" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G630" s="13"/>
       <c r="H630" s="13"/>
     </row>
-    <row r="631" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="631" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G631" s="13"/>
       <c r="H631" s="13"/>
     </row>
-    <row r="632" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="632" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G632" s="13"/>
       <c r="H632" s="13"/>
     </row>
-    <row r="633" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="633" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G633" s="13"/>
       <c r="H633" s="13"/>
     </row>
-    <row r="634" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="634" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G634" s="13"/>
       <c r="H634" s="13"/>
     </row>
-    <row r="635" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="635" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G635" s="13"/>
       <c r="H635" s="13"/>
     </row>
-    <row r="636" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="636" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G636" s="13"/>
       <c r="H636" s="13"/>
     </row>
-    <row r="637" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="637" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G637" s="13"/>
       <c r="H637" s="13"/>
     </row>
-    <row r="638" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="638" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G638" s="13"/>
       <c r="H638" s="13"/>
     </row>
-    <row r="639" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="639" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G639" s="13"/>
       <c r="H639" s="13"/>
     </row>
-    <row r="640" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="640" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G640" s="13"/>
       <c r="H640" s="13"/>
     </row>
-    <row r="641" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="641" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G641" s="13"/>
       <c r="H641" s="13"/>
     </row>
-    <row r="642" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="642" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G642" s="13"/>
       <c r="H642" s="13"/>
     </row>
-    <row r="643" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="643" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G643" s="13"/>
       <c r="H643" s="13"/>
     </row>
-    <row r="644" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="644" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G644" s="13"/>
       <c r="H644" s="13"/>
     </row>
-    <row r="645" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="645" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G645" s="13"/>
       <c r="H645" s="13"/>
     </row>
-    <row r="646" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="646" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G646" s="13"/>
       <c r="H646" s="13"/>
     </row>
-    <row r="647" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="647" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G647" s="13"/>
       <c r="H647" s="13"/>
     </row>
-    <row r="648" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="648" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G648" s="13"/>
       <c r="H648" s="13"/>
     </row>
-    <row r="649" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="649" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G649" s="13"/>
       <c r="H649" s="13"/>
     </row>
-    <row r="650" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="650" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G650" s="13"/>
       <c r="H650" s="13"/>
     </row>
-    <row r="651" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="651" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G651" s="13"/>
       <c r="H651" s="13"/>
     </row>
-    <row r="652" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="652" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G652" s="13"/>
       <c r="H652" s="13"/>
     </row>
-    <row r="653" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="653" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G653" s="13"/>
       <c r="H653" s="13"/>
     </row>
-    <row r="654" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="654" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G654" s="13"/>
       <c r="H654" s="13"/>
     </row>
-    <row r="655" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="655" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G655" s="13"/>
       <c r="H655" s="13"/>
     </row>
-    <row r="656" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="656" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G656" s="13"/>
       <c r="H656" s="13"/>
     </row>
-    <row r="657" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="657" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G657" s="13"/>
       <c r="H657" s="13"/>
     </row>
-    <row r="658" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="658" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G658" s="13"/>
       <c r="H658" s="13"/>
     </row>
-    <row r="659" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="659" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G659" s="13"/>
       <c r="H659" s="13"/>
     </row>
-    <row r="660" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="660" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G660" s="13"/>
       <c r="H660" s="13"/>
     </row>
-    <row r="661" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="661" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G661" s="13"/>
       <c r="H661" s="13"/>
     </row>
-    <row r="662" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="662" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G662" s="13"/>
       <c r="H662" s="13"/>
     </row>
-    <row r="663" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="663" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G663" s="13"/>
       <c r="H663" s="13"/>
     </row>
-    <row r="664" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="664" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G664" s="13"/>
       <c r="H664" s="13"/>
     </row>
-    <row r="665" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="665" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G665" s="13"/>
       <c r="H665" s="13"/>
     </row>
-    <row r="666" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="666" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G666" s="13"/>
       <c r="H666" s="13"/>
     </row>
-    <row r="667" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="667" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G667" s="13"/>
       <c r="H667" s="13"/>
     </row>
-    <row r="668" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="668" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G668" s="13"/>
       <c r="H668" s="13"/>
     </row>
-    <row r="669" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="669" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G669" s="13"/>
       <c r="H669" s="13"/>
     </row>
-    <row r="670" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="670" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G670" s="13"/>
       <c r="H670" s="13"/>
     </row>
-    <row r="671" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="671" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G671" s="13"/>
       <c r="H671" s="13"/>
     </row>
-    <row r="672" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="672" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G672" s="13"/>
       <c r="H672" s="13"/>
     </row>
-    <row r="673" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="673" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G673" s="13"/>
       <c r="H673" s="13"/>
     </row>
-    <row r="674" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="674" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G674" s="13"/>
       <c r="H674" s="13"/>
     </row>
-    <row r="675" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="675" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G675" s="13"/>
       <c r="H675" s="13"/>
     </row>
-    <row r="676" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="676" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G676" s="13"/>
       <c r="H676" s="13"/>
     </row>
-    <row r="677" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="677" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G677" s="13"/>
       <c r="H677" s="13"/>
     </row>
-    <row r="678" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="678" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G678" s="13"/>
       <c r="H678" s="13"/>
     </row>
-    <row r="679" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="679" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G679" s="13"/>
       <c r="H679" s="13"/>
     </row>
-    <row r="680" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="680" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G680" s="13"/>
       <c r="H680" s="13"/>
     </row>
-    <row r="681" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="681" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G681" s="13"/>
       <c r="H681" s="13"/>
     </row>
-    <row r="682" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="682" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G682" s="13"/>
       <c r="H682" s="13"/>
     </row>
-    <row r="683" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="683" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G683" s="13"/>
       <c r="H683" s="13"/>
     </row>
-    <row r="684" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="684" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G684" s="13"/>
       <c r="H684" s="13"/>
     </row>
-    <row r="685" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="685" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G685" s="13"/>
       <c r="H685" s="13"/>
     </row>
-    <row r="686" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="686" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G686" s="13"/>
       <c r="H686" s="13"/>
     </row>
-    <row r="687" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="687" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G687" s="13"/>
       <c r="H687" s="13"/>
     </row>
-    <row r="688" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="688" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G688" s="13"/>
       <c r="H688" s="13"/>
     </row>
-    <row r="689" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="689" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G689" s="13"/>
       <c r="H689" s="13"/>
     </row>
-    <row r="690" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="690" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G690" s="13"/>
       <c r="H690" s="13"/>
     </row>
-    <row r="691" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="691" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G691" s="13"/>
       <c r="H691" s="13"/>
     </row>
-    <row r="692" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="692" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G692" s="13"/>
       <c r="H692" s="13"/>
     </row>
-    <row r="693" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="693" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G693" s="13"/>
       <c r="H693" s="13"/>
     </row>
-    <row r="694" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="694" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G694" s="13"/>
       <c r="H694" s="13"/>
     </row>
-    <row r="695" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="695" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G695" s="13"/>
       <c r="H695" s="13"/>
     </row>
-    <row r="696" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="696" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G696" s="13"/>
       <c r="H696" s="13"/>
     </row>
-    <row r="697" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="697" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G697" s="13"/>
       <c r="H697" s="13"/>
     </row>
-    <row r="698" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="698" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G698" s="13"/>
       <c r="H698" s="13"/>
     </row>
-    <row r="699" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="699" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G699" s="13"/>
       <c r="H699" s="13"/>
     </row>
-    <row r="700" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="700" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G700" s="13"/>
       <c r="H700" s="13"/>
     </row>
-    <row r="701" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="701" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G701" s="13"/>
       <c r="H701" s="13"/>
     </row>
-    <row r="702" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="702" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G702" s="13"/>
       <c r="H702" s="13"/>
     </row>
-    <row r="703" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="703" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G703" s="13"/>
       <c r="H703" s="13"/>
     </row>
-    <row r="704" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="704" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G704" s="13"/>
       <c r="H704" s="13"/>
     </row>
-    <row r="705" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="705" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G705" s="13"/>
       <c r="H705" s="13"/>
     </row>
-    <row r="706" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="706" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G706" s="13"/>
       <c r="H706" s="13"/>
     </row>
-    <row r="707" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="707" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G707" s="13"/>
       <c r="H707" s="13"/>
     </row>
-    <row r="708" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="708" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G708" s="13"/>
       <c r="H708" s="13"/>
     </row>
-    <row r="709" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="709" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G709" s="13"/>
       <c r="H709" s="13"/>
     </row>
-    <row r="710" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="710" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G710" s="13"/>
       <c r="H710" s="13"/>
     </row>
-    <row r="711" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="711" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G711" s="13"/>
       <c r="H711" s="13"/>
     </row>
-    <row r="712" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="712" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G712" s="13"/>
       <c r="H712" s="13"/>
     </row>
-    <row r="713" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="713" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G713" s="13"/>
       <c r="H713" s="13"/>
     </row>
-    <row r="714" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="714" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G714" s="13"/>
       <c r="H714" s="13"/>
     </row>
-    <row r="715" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="715" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G715" s="13"/>
       <c r="H715" s="13"/>
     </row>
-    <row r="716" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="716" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G716" s="13"/>
       <c r="H716" s="13"/>
     </row>
-    <row r="717" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="717" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G717" s="13"/>
       <c r="H717" s="13"/>
     </row>
-    <row r="718" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="718" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G718" s="13"/>
       <c r="H718" s="13"/>
     </row>
-    <row r="719" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="719" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G719" s="13"/>
       <c r="H719" s="13"/>
     </row>
-    <row r="720" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="720" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G720" s="13"/>
       <c r="H720" s="13"/>
     </row>
-    <row r="721" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="721" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G721" s="13"/>
       <c r="H721" s="13"/>
     </row>
-    <row r="722" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="722" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G722" s="13"/>
       <c r="H722" s="25"/>
     </row>
-    <row r="723" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="723" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G723" s="13"/>
       <c r="H723" s="25"/>
     </row>
-    <row r="724" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="724" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G724" s="13"/>
       <c r="H724" s="25"/>
     </row>
-    <row r="725" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="725" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G725" s="13"/>
       <c r="H725" s="25"/>
     </row>
-    <row r="726" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="726" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G726" s="13"/>
       <c r="H726" s="25"/>
     </row>
-    <row r="727" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="727" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G727" s="13"/>
       <c r="H727" s="25"/>
     </row>
-    <row r="728" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="728" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G728" s="13"/>
       <c r="H728" s="25"/>
     </row>
-    <row r="729" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="729" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G729" s="13"/>
       <c r="H729" s="25"/>
     </row>
-    <row r="730" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="730" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G730" s="13"/>
       <c r="H730" s="25"/>
     </row>
-    <row r="731" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="731" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G731" s="13"/>
       <c r="H731" s="25"/>
     </row>
-    <row r="732" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="732" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G732" s="13"/>
       <c r="H732" s="25"/>
     </row>
-    <row r="733" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="733" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G733" s="13"/>
       <c r="H733" s="25"/>
     </row>
-    <row r="734" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="734" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G734" s="13"/>
       <c r="H734" s="25"/>
     </row>
-    <row r="735" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="735" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G735" s="13"/>
       <c r="H735" s="25"/>
     </row>
-    <row r="736" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="736" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G736" s="13"/>
       <c r="H736" s="25"/>
     </row>
-    <row r="737" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="737" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G737" s="13"/>
       <c r="H737" s="25"/>
     </row>
-    <row r="738" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="738" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G738" s="13"/>
       <c r="H738" s="25"/>
     </row>
-    <row r="739" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="739" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G739" s="13"/>
       <c r="H739" s="25"/>
     </row>
-    <row r="740" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="740" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G740" s="13"/>
       <c r="H740" s="25"/>
     </row>
-    <row r="741" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="741" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G741" s="13"/>
       <c r="H741" s="25"/>
     </row>
-    <row r="742" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="742" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G742" s="13"/>
       <c r="H742" s="25"/>
     </row>
-    <row r="743" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="743" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G743" s="13"/>
       <c r="H743" s="25"/>
     </row>
-    <row r="744" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="744" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G744" s="13"/>
       <c r="H744" s="25"/>
     </row>
-    <row r="745" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="745" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G745" s="13"/>
       <c r="H745" s="25"/>
     </row>
-    <row r="746" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="746" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G746" s="13"/>
       <c r="H746" s="25"/>
     </row>
-    <row r="747" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="747" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G747" s="13"/>
       <c r="H747" s="25"/>
     </row>
-    <row r="748" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="748" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G748" s="13"/>
       <c r="H748" s="25"/>
     </row>
-    <row r="749" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="749" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G749" s="13"/>
       <c r="H749" s="25"/>
     </row>
-    <row r="750" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="750" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G750" s="13"/>
       <c r="H750" s="25"/>
     </row>
-    <row r="751" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="751" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G751" s="13"/>
       <c r="H751" s="25"/>
     </row>
-    <row r="752" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="752" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G752" s="13"/>
       <c r="H752" s="25"/>
     </row>
-    <row r="753" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="753" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G753" s="13"/>
       <c r="H753" s="25"/>
     </row>
-    <row r="754" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="754" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G754" s="13"/>
       <c r="H754" s="25"/>
     </row>
-    <row r="755" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="755" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G755" s="13"/>
       <c r="H755" s="25"/>
     </row>
-    <row r="756" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="756" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G756" s="13"/>
       <c r="H756" s="25"/>
     </row>
-    <row r="757" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="757" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G757" s="13"/>
       <c r="H757" s="25"/>
     </row>
-    <row r="758" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="758" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G758" s="13"/>
       <c r="H758" s="25"/>
     </row>
-    <row r="759" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="759" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H759" s="20"/>
     </row>
-    <row r="760" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="760" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H760" s="20"/>
     </row>
-    <row r="761" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="761" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H761" s="20"/>
     </row>
-    <row r="762" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="762" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H762" s="20"/>
     </row>
-    <row r="763" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="763" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H763" s="20"/>
     </row>
-    <row r="764" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="764" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H764" s="20"/>
     </row>
-    <row r="765" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="765" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H765" s="20"/>
     </row>
-    <row r="766" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="766" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H766" s="20"/>
     </row>
-    <row r="767" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="767" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H767" s="20"/>
     </row>
-    <row r="768" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="768" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H768" s="20"/>
     </row>
-    <row r="769" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="769" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H769" s="20"/>
     </row>
-    <row r="770" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="770" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H770" s="20"/>
     </row>
-    <row r="771" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="771" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H771" s="20"/>
     </row>
-    <row r="772" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="772" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H772" s="20"/>
     </row>
-    <row r="773" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="773" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H773" s="20"/>
     </row>
-    <row r="774" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="774" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H774" s="20"/>
     </row>
-    <row r="775" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="775" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H775" s="20"/>
     </row>
-    <row r="776" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="776" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H776" s="20"/>
     </row>
-    <row r="777" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="777" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H777" s="20"/>
     </row>
-    <row r="798" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="798" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G798" s="14"/>
       <c r="H798" s="14"/>
     </row>
-    <row r="799" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="799" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G799" s="14"/>
       <c r="H799" s="14"/>
     </row>
-    <row r="800" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="800" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G800" s="14"/>
       <c r="H800" s="14"/>
     </row>
-    <row r="801" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="801" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G801" s="14"/>
       <c r="H801" s="14"/>
     </row>
-    <row r="802" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="802" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G802" s="14"/>
       <c r="H802" s="14"/>
     </row>
-    <row r="803" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="803" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G803" s="14"/>
       <c r="H803" s="14"/>
     </row>
-    <row r="804" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="804" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G804" s="14"/>
       <c r="H804" s="14"/>
     </row>
-    <row r="805" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="805" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G805" s="14"/>
       <c r="H805" s="14"/>
     </row>
-    <row r="806" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="806" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G806" s="14"/>
       <c r="H806" s="14"/>
     </row>
-    <row r="807" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="807" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G807" s="14"/>
       <c r="H807" s="14"/>
     </row>
-    <row r="808" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="808" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G808" s="14"/>
       <c r="H808" s="14"/>
     </row>
-    <row r="809" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="809" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G809" s="14"/>
       <c r="H809" s="14"/>
     </row>
-    <row r="818" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="818" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G818" s="14"/>
       <c r="H818" s="14"/>
     </row>
-    <row r="819" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="819" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G819" s="14"/>
       <c r="H819" s="14"/>
     </row>
-    <row r="820" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="820" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G820" s="14"/>
       <c r="H820" s="14"/>
     </row>
-    <row r="821" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="821" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G821" s="14"/>
       <c r="H821" s="14"/>
     </row>
-    <row r="822" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="822" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G822" s="14"/>
       <c r="H822" s="21"/>
     </row>
-    <row r="823" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="823" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G823" s="14"/>
       <c r="H823" s="21"/>
     </row>
-    <row r="824" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="824" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G824" s="14"/>
       <c r="H824" s="21"/>
     </row>
-    <row r="825" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="825" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G825" s="14"/>
       <c r="H825" s="21"/>
     </row>
-    <row r="826" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="826" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G826" s="14"/>
       <c r="H826" s="21"/>
     </row>
-    <row r="827" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="827" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G827" s="14"/>
       <c r="H827" s="14"/>
     </row>
-    <row r="828" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="828" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G828" s="14"/>
       <c r="H828" s="14"/>
     </row>
-    <row r="829" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="829" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G829" s="14"/>
       <c r="H829" s="14"/>
     </row>
-    <row r="830" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="830" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G830" s="14"/>
       <c r="H830" s="14"/>
     </row>
-    <row r="831" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="831" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G831" s="14"/>
       <c r="H831" s="14"/>
     </row>
-    <row r="832" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="832" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G832" s="14"/>
       <c r="H832" s="14"/>
     </row>
-    <row r="833" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="833" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G833" s="14"/>
       <c r="H833" s="14"/>
     </row>
-    <row r="834" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="834" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G834" s="14"/>
       <c r="H834" s="14"/>
     </row>
-    <row r="835" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="835" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G835" s="14"/>
       <c r="H835" s="14"/>
     </row>
-    <row r="836" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="836" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G836" s="14"/>
       <c r="H836" s="14"/>
     </row>
-    <row r="837" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="837" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G837" s="14"/>
       <c r="H837" s="14"/>
     </row>
-    <row r="838" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="838" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G838" s="14"/>
       <c r="H838" s="14"/>
     </row>
-    <row r="842" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="842" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H842" s="22"/>
     </row>
-    <row r="847" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="847" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G847" s="14"/>
       <c r="H847" s="14"/>
     </row>
-    <row r="848" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="848" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G848" s="14"/>
       <c r="H848" s="14"/>
     </row>
-    <row r="849" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="849" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G849" s="14"/>
       <c r="H849" s="14"/>
     </row>
-    <row r="850" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="850" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G850" s="14"/>
       <c r="H850" s="14"/>
     </row>
-    <row r="851" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="851" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G851" s="14"/>
       <c r="H851" s="21"/>
     </row>
-    <row r="852" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="852" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G852" s="14"/>
       <c r="H852" s="21"/>
     </row>
-    <row r="853" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="853" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G853" s="14"/>
       <c r="H853" s="21"/>
     </row>
-    <row r="854" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="854" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G854" s="14"/>
       <c r="H854" s="21"/>
     </row>
-    <row r="855" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="855" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G855" s="14"/>
       <c r="H855" s="21"/>
     </row>
-    <row r="856" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="856" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G856" s="14"/>
       <c r="H856" s="14"/>
     </row>
-    <row r="857" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="857" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G857" s="14"/>
       <c r="H857" s="14"/>
     </row>
-    <row r="858" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="858" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G858" s="14"/>
       <c r="H858" s="14"/>
     </row>
-    <row r="859" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="859" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G859" s="14"/>
       <c r="H859" s="14"/>
     </row>
-    <row r="860" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="860" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G860" s="14"/>
       <c r="H860" s="14"/>
     </row>
-    <row r="861" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="861" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G861" s="14"/>
       <c r="H861" s="14"/>
     </row>
-    <row r="862" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="862" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G862" s="14"/>
       <c r="H862" s="14"/>
     </row>
-    <row r="863" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="863" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G863" s="14"/>
       <c r="H863" s="14"/>
     </row>
-    <row r="864" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="864" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G864" s="14"/>
       <c r="H864" s="14"/>
     </row>
-    <row r="865" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="865" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G865" s="14"/>
       <c r="H865" s="14"/>
     </row>
-    <row r="866" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="866" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G866" s="14"/>
       <c r="H866" s="14"/>
     </row>
-    <row r="867" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="867" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G867" s="14"/>
       <c r="H867" s="14"/>
     </row>
-    <row r="871" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="871" spans="7:8" x14ac:dyDescent="0.2">
       <c r="H871" s="22"/>
     </row>
-    <row r="876" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="876" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G876" s="14"/>
       <c r="H876" s="14"/>
     </row>
-    <row r="877" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="877" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G877" s="14"/>
       <c r="H877" s="14"/>
     </row>
-    <row r="878" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="878" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G878" s="14"/>
       <c r="H878" s="14"/>
     </row>
-    <row r="879" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="879" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G879" s="14"/>
       <c r="H879" s="14"/>
     </row>
-    <row r="880" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="880" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G880" s="14"/>
       <c r="H880" s="21"/>
     </row>
-    <row r="881" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="881" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G881" s="14"/>
       <c r="H881" s="21"/>
     </row>
-    <row r="882" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="882" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G882" s="14"/>
       <c r="H882" s="21"/>
     </row>
-    <row r="883" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="883" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G883" s="14"/>
       <c r="H883" s="21"/>
     </row>
-    <row r="884" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="884" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G884" s="14"/>
       <c r="H884" s="21"/>
     </row>
-    <row r="942" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="942" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H942" s="11"/>
     </row>
-    <row r="943" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="943" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H943" s="11"/>
     </row>
-    <row r="944" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="944" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H944" s="11"/>
     </row>
-    <row r="945" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="945" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H945" s="11"/>
     </row>
-    <row r="946" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="946" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H946" s="11"/>
     </row>
-    <row r="947" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="947" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H947" s="11"/>
     </row>
-    <row r="948" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="948" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H948" s="11"/>
     </row>
-    <row r="949" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="949" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H949" s="11"/>
     </row>
-    <row r="950" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="950" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H950" s="11"/>
     </row>
-    <row r="951" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="951" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H951" s="11"/>
     </row>
-    <row r="952" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="952" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H952" s="11"/>
     </row>
-    <row r="953" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="953" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H953" s="11"/>
     </row>
-    <row r="954" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="954" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H954" s="12"/>
     </row>
-    <row r="955" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="955" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H955" s="12"/>
     </row>
-    <row r="956" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="956" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H956" s="12"/>
     </row>
-    <row r="957" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="957" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H957" s="12"/>
     </row>
-    <row r="958" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="958" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H958" s="12"/>
     </row>
-    <row r="959" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="959" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H959" s="12"/>
     </row>
-    <row r="960" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="960" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H960" s="12"/>
     </row>
-    <row r="961" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="961" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H961" s="12"/>
     </row>
-    <row r="962" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="962" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H962" s="12"/>
     </row>
-    <row r="963" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="963" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H963" s="12"/>
     </row>
-    <row r="964" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="964" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H964" s="23"/>
     </row>
-    <row r="965" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="965" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H965" s="12"/>
     </row>
-    <row r="966" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="966" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H966" s="12"/>
     </row>
-    <row r="967" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="967" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H967" s="24"/>
     </row>
-    <row r="968" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="968" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H968" s="12"/>
     </row>
-    <row r="969" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="969" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H969" s="12"/>
     </row>
-    <row r="970" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="970" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H970" s="12"/>
     </row>
-    <row r="971" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="971" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H971" s="12"/>
     </row>
-    <row r="972" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="972" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H972" s="12"/>
     </row>
-    <row r="1037" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1037" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1037" s="26"/>
       <c r="H1037" s="6"/>
     </row>
-    <row r="1038" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1038" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1038" s="26"/>
       <c r="H1038" s="6"/>
     </row>
-    <row r="1039" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1039" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1039" s="26"/>
       <c r="H1039" s="6"/>
     </row>
-    <row r="1040" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1040" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1040" s="26"/>
       <c r="H1040" s="6"/>
     </row>
-    <row r="1041" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1041" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1041" s="26"/>
       <c r="H1041" s="6"/>
     </row>
-    <row r="1042" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1042" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1042" s="26"/>
       <c r="H1042" s="6"/>
     </row>
-    <row r="1043" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1043" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1043" s="26"/>
       <c r="H1043" s="6"/>
     </row>
-    <row r="1044" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1044" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1044" s="26"/>
       <c r="H1044" s="6"/>
     </row>
-    <row r="1045" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1045" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1045" s="26"/>
       <c r="H1045" s="6"/>
     </row>
-    <row r="1046" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1046" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1046" s="26"/>
       <c r="H1046" s="6"/>
     </row>
-    <row r="1047" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1047" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1047" s="26"/>
       <c r="H1047" s="6"/>
     </row>
-    <row r="1048" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1048" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1048" s="26"/>
       <c r="H1048" s="6"/>
     </row>
-    <row r="1049" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1049" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1049" s="26"/>
       <c r="H1049" s="6"/>
     </row>
-    <row r="1050" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1050" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1050" s="26"/>
       <c r="H1050" s="6"/>
     </row>
-    <row r="1051" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1051" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1051" s="26"/>
       <c r="H1051" s="6"/>
     </row>
-    <row r="1052" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1052" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1052" s="26"/>
       <c r="H1052" s="6"/>
     </row>
-    <row r="1053" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1053" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1053" s="26"/>
       <c r="H1053" s="6"/>
     </row>
-    <row r="1054" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1054" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1054" s="26"/>
       <c r="H1054" s="6"/>
     </row>
-    <row r="1055" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1055" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1055" s="26"/>
       <c r="H1055" s="6"/>
     </row>
-    <row r="1056" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1056" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1056" s="26"/>
       <c r="H1056" s="6"/>
     </row>
-    <row r="1057" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1057" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1057" s="26"/>
       <c r="H1057" s="6"/>
     </row>
-    <row r="1058" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1058" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1058" s="26"/>
       <c r="H1058" s="6"/>
     </row>
-    <row r="1059" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1059" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1059" s="26"/>
       <c r="H1059" s="6"/>
     </row>
-    <row r="1060" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1060" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1060" s="26"/>
       <c r="H1060" s="6"/>
     </row>
-    <row r="1061" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1061" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1061" s="26"/>
       <c r="H1061" s="6"/>
     </row>
-    <row r="1062" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1062" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1062" s="26"/>
       <c r="H1062" s="6"/>
     </row>
-    <row r="1063" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1063" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1063" s="26"/>
       <c r="H1063" s="6"/>
     </row>
-    <row r="1064" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1064" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1064" s="26"/>
       <c r="H1064" s="6"/>
     </row>
-    <row r="1065" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1065" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1065" s="26"/>
       <c r="H1065" s="6"/>
     </row>
-    <row r="1066" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1066" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1066" s="26"/>
       <c r="H1066" s="6"/>
     </row>
-    <row r="1067" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1067" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1067" s="26"/>
       <c r="H1067" s="6"/>
     </row>
-    <row r="1068" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1068" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1068" s="26"/>
       <c r="H1068" s="6"/>
     </row>
-    <row r="1069" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1069" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1069" s="26"/>
       <c r="H1069" s="6"/>
     </row>
-    <row r="1070" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1070" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1070" s="26"/>
       <c r="H1070" s="6"/>
     </row>
-    <row r="1071" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1071" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1071" s="26"/>
       <c r="H1071" s="6"/>
     </row>
-    <row r="1072" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1072" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1072" s="26"/>
       <c r="H1072" s="6"/>
     </row>
-    <row r="1073" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1073" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1073" s="26"/>
       <c r="H1073" s="6"/>
     </row>
-    <row r="1074" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1074" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1074" s="26"/>
       <c r="H1074" s="6"/>
     </row>
-    <row r="1075" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1075" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1075" s="26"/>
       <c r="H1075" s="6"/>
     </row>
-    <row r="1076" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1076" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1076" s="26"/>
       <c r="H1076" s="6"/>
     </row>
-    <row r="1077" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1077" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1077" s="26"/>
       <c r="H1077" s="6"/>
     </row>
-    <row r="1078" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1078" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1078" s="26"/>
       <c r="H1078" s="6"/>
     </row>
-    <row r="1079" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1079" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1079" s="26"/>
       <c r="H1079" s="6"/>
     </row>
-    <row r="1080" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1080" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1080" s="26"/>
       <c r="H1080" s="6"/>
     </row>
-    <row r="1081" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1081" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1081" s="26"/>
       <c r="H1081" s="6"/>
     </row>
-    <row r="1082" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1082" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1082" s="26"/>
       <c r="H1082" s="6"/>
     </row>
-    <row r="1083" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1083" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1083" s="26"/>
       <c r="H1083" s="6"/>
     </row>
-    <row r="1084" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1084" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1084" s="26"/>
       <c r="H1084" s="6"/>
     </row>
-    <row r="1085" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1085" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1085" s="26"/>
       <c r="H1085" s="27"/>
     </row>
-    <row r="1086" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1086" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1086" s="26"/>
       <c r="H1086" s="27"/>
     </row>
-    <row r="1087" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1087" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1087" s="26"/>
       <c r="H1087" s="6"/>
     </row>
-    <row r="1088" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1088" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1088" s="26"/>
       <c r="H1088" s="6"/>
     </row>
-    <row r="1089" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1089" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1089" s="26"/>
       <c r="H1089" s="6"/>
     </row>
-    <row r="1090" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1090" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1090" s="26"/>
       <c r="H1090" s="6"/>
     </row>
-    <row r="1091" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1091" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1091" s="26"/>
       <c r="H1091" s="6"/>
     </row>
-    <row r="1092" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1092" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1092" s="26"/>
       <c r="H1092" s="6"/>
     </row>
-    <row r="1093" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1093" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1093" s="26"/>
       <c r="H1093" s="6"/>
     </row>
-    <row r="1094" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1094" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1094" s="26"/>
       <c r="H1094" s="6"/>
     </row>
-    <row r="1095" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1095" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1095" s="26"/>
       <c r="H1095" s="6"/>
     </row>
-    <row r="1096" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1096" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1096" s="26"/>
       <c r="H1096" s="6"/>
     </row>
-    <row r="1097" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1097" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1097" s="26"/>
       <c r="H1097" s="6"/>
     </row>
-    <row r="1098" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1098" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1098" s="26"/>
       <c r="H1098" s="6"/>
     </row>
-    <row r="1099" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1099" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1099" s="26"/>
       <c r="H1099" s="6"/>
     </row>
-    <row r="1100" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1100" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1100" s="26"/>
       <c r="H1100" s="6"/>
     </row>
-    <row r="1101" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1101" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1101" s="26"/>
       <c r="H1101" s="6"/>
     </row>
-    <row r="1102" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1102" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1102" s="26"/>
       <c r="H1102" s="6"/>
     </row>
-    <row r="1103" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1103" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1103" s="26"/>
       <c r="H1103" s="6"/>
     </row>
-    <row r="1104" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1104" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1104" s="26"/>
       <c r="H1104" s="6"/>
     </row>
-    <row r="1105" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1105" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1105" s="26"/>
       <c r="H1105" s="6"/>
     </row>
-    <row r="1106" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1106" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1106" s="26"/>
       <c r="H1106" s="6"/>
     </row>
-    <row r="1107" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1107" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1107" s="26"/>
       <c r="H1107" s="6"/>
     </row>
-    <row r="1108" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1108" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1108" s="28"/>
       <c r="G1108" s="26"/>
       <c r="H1108" s="6"/>
     </row>
-    <row r="1109" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1109" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1109" s="28"/>
       <c r="G1109" s="26"/>
       <c r="H1109" s="6"/>
     </row>
-    <row r="1110" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1110" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1110" s="28"/>
       <c r="G1110" s="26"/>
       <c r="H1110" s="6"/>
     </row>
-    <row r="1111" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1111" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1111" s="28"/>
       <c r="G1111" s="26"/>
       <c r="H1111" s="6"/>
     </row>
-    <row r="1112" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1112" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1112" s="28"/>
       <c r="G1112" s="26"/>
       <c r="H1112" s="6"/>
     </row>
-    <row r="1113" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1113" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1113" s="28"/>
       <c r="G1113" s="26"/>
       <c r="H1113" s="6"/>
     </row>
-    <row r="1114" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1114" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1114" s="28"/>
       <c r="G1114" s="26"/>
       <c r="H1114" s="6"/>
     </row>
-    <row r="1115" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1115" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1115" s="28"/>
       <c r="G1115" s="26"/>
       <c r="H1115" s="6"/>
     </row>
-    <row r="1116" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1116" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1116" s="28"/>
       <c r="G1116" s="26"/>
       <c r="H1116" s="6"/>
     </row>
-    <row r="1117" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1117" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1117" s="28"/>
       <c r="G1117" s="26"/>
       <c r="H1117" s="6"/>
     </row>
-    <row r="1118" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1118" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1118" s="28"/>
       <c r="G1118" s="26"/>
       <c r="H1118" s="6"/>
     </row>
-    <row r="1119" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1119" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1119" s="28"/>
       <c r="G1119" s="26"/>
       <c r="H1119" s="6"/>
     </row>
-    <row r="1120" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1120" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1120" s="28"/>
       <c r="G1120" s="26"/>
       <c r="H1120" s="6"/>
     </row>
-    <row r="1121" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1121" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1121" s="28"/>
       <c r="G1121" s="26"/>
       <c r="H1121" s="6"/>
     </row>
-    <row r="1122" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1122" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1122" s="28"/>
       <c r="G1122" s="26"/>
       <c r="H1122" s="6"/>
     </row>
-    <row r="1123" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1123" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1123" s="28"/>
       <c r="G1123" s="26"/>
       <c r="H1123" s="6"/>
     </row>
-    <row r="1124" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1124" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1124" s="28"/>
       <c r="G1124" s="26"/>
       <c r="H1124" s="6"/>
     </row>
-    <row r="1125" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1125" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1125" s="28"/>
       <c r="G1125" s="26"/>
       <c r="H1125" s="6"/>
     </row>
-    <row r="1126" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1126" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1126" s="28"/>
       <c r="G1126" s="26"/>
       <c r="H1126" s="6"/>
     </row>
-    <row r="1127" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1127" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1127" s="28"/>
       <c r="G1127" s="26"/>
       <c r="H1127" s="6"/>
     </row>
-    <row r="1128" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1128" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1128" s="28"/>
       <c r="G1128" s="26"/>
       <c r="H1128" s="6"/>
     </row>
-    <row r="1129" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1129" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1129" s="28"/>
       <c r="G1129" s="26"/>
       <c r="H1129" s="6"/>
     </row>
-    <row r="1130" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1130" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1130" s="28"/>
       <c r="G1130" s="26"/>
       <c r="H1130" s="6"/>
     </row>
-    <row r="1131" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1131" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1131" s="28"/>
       <c r="G1131" s="26"/>
       <c r="H1131" s="6"/>
     </row>
-    <row r="1132" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1132" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1132" s="28"/>
       <c r="G1132" s="26"/>
       <c r="H1132" s="6"/>
     </row>
-    <row r="1133" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1133" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1133" s="28"/>
       <c r="G1133" s="26"/>
       <c r="H1133" s="6"/>
     </row>
-    <row r="1134" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1134" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1134" s="28"/>
       <c r="G1134" s="26"/>
       <c r="H1134" s="6"/>
     </row>
-    <row r="1135" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1135" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1135" s="28"/>
       <c r="G1135" s="26"/>
       <c r="H1135" s="6"/>
     </row>
-    <row r="1136" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1136" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1136" s="28"/>
       <c r="G1136" s="26"/>
       <c r="H1136" s="6"/>
     </row>
-    <row r="1137" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1137" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1137" s="28"/>
       <c r="G1137" s="26"/>
       <c r="H1137" s="6"/>
     </row>
-    <row r="1138" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1138" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1138" s="28"/>
       <c r="G1138" s="26"/>
       <c r="H1138" s="6"/>
     </row>
-    <row r="1139" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1139" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1139" s="28"/>
       <c r="G1139" s="26"/>
       <c r="H1139" s="6"/>
     </row>
-    <row r="1140" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1140" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1140" s="28"/>
       <c r="G1140" s="26"/>
       <c r="H1140" s="6"/>
     </row>
-    <row r="1141" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1141" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1141" s="28"/>
       <c r="G1141" s="26"/>
       <c r="H1141" s="6"/>
     </row>
-    <row r="1142" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1142" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1142" s="28"/>
       <c r="G1142" s="26"/>
       <c r="H1142" s="27"/>
     </row>
-    <row r="1143" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1143" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1143" s="28"/>
       <c r="G1143" s="26"/>
       <c r="H1143" s="27"/>
     </row>
-    <row r="1144" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1144" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1144" s="28"/>
       <c r="G1144" s="26"/>
       <c r="H1144" s="6"/>
     </row>
-    <row r="1145" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1145" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1145" s="28"/>
       <c r="G1145" s="26"/>
       <c r="H1145" s="6"/>
     </row>
-    <row r="1146" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1146" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1146" s="28"/>
       <c r="G1146" s="26"/>
       <c r="H1146" s="6"/>
     </row>
-    <row r="1147" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1147" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1147" s="28"/>
       <c r="G1147" s="26"/>
       <c r="H1147" s="6"/>
     </row>
-    <row r="1148" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1148" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1148" s="28"/>
       <c r="G1148" s="26"/>
       <c r="H1148" s="6"/>
     </row>
-    <row r="1149" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1149" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1149" s="28"/>
       <c r="G1149" s="26"/>
       <c r="H1149" s="6"/>
     </row>
-    <row r="1150" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1150" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1150" s="28"/>
       <c r="G1150" s="26"/>
       <c r="H1150" s="6"/>
     </row>
-    <row r="1151" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1151" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1151" s="28"/>
       <c r="G1151" s="26"/>
       <c r="H1151" s="6"/>
     </row>
-    <row r="1152" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1152" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1152" s="28"/>
       <c r="G1152" s="26"/>
       <c r="H1152" s="6"/>
     </row>
-    <row r="1153" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1153" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1153" s="28"/>
       <c r="G1153" s="26"/>
       <c r="H1153" s="6"/>
     </row>
-    <row r="1154" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1154" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1154" s="28"/>
       <c r="G1154" s="26"/>
       <c r="H1154" s="6"/>
     </row>
-    <row r="1155" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1155" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1155" s="28"/>
       <c r="G1155" s="26"/>
       <c r="H1155" s="6"/>
     </row>
-    <row r="1156" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1156" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1156" s="28"/>
       <c r="G1156" s="26"/>
       <c r="H1156" s="6"/>
     </row>
-    <row r="1157" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1157" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1157" s="28"/>
       <c r="G1157" s="26"/>
       <c r="H1157" s="6"/>
     </row>
-    <row r="1158" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1158" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1158" s="28"/>
       <c r="G1158" s="26"/>
       <c r="H1158" s="6"/>
     </row>
-    <row r="1159" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1159" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1159" s="28"/>
       <c r="G1159" s="26"/>
       <c r="H1159" s="6"/>
     </row>
-    <row r="1160" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1160" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1160" s="28"/>
       <c r="G1160" s="26"/>
       <c r="H1160" s="6"/>
     </row>
-    <row r="1161" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1161" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1161" s="28"/>
       <c r="G1161" s="26"/>
       <c r="H1161" s="6"/>
     </row>
-    <row r="1162" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1162" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1162" s="28"/>
       <c r="G1162" s="26"/>
       <c r="H1162" s="6"/>
     </row>
-    <row r="1163" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1163" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1163" s="28"/>
       <c r="G1163" s="26"/>
       <c r="H1163" s="6"/>
     </row>
-    <row r="1164" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1164" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D1164" s="28"/>
       <c r="G1164" s="26"/>
       <c r="H1164" s="6"/>
     </row>
-    <row r="1165" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1165" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1165" s="26"/>
       <c r="H1165" s="27"/>
     </row>
-    <row r="1166" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1166" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1166" s="26"/>
       <c r="H1166" s="6"/>
     </row>
-    <row r="1167" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1167" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1167" s="26"/>
       <c r="H1167" s="6"/>
     </row>
-    <row r="1168" spans="4:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1168" spans="4:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1168" s="26"/>
       <c r="H1168" s="6"/>
     </row>
-    <row r="1169" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1169" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1169" s="26"/>
       <c r="H1169" s="6"/>
     </row>
-    <row r="1170" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1170" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1170" s="26"/>
       <c r="H1170" s="6"/>
     </row>
-    <row r="1171" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1171" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1171" s="26"/>
       <c r="H1171" s="6"/>
     </row>
-    <row r="1172" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1172" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1172" s="26"/>
       <c r="H1172" s="6"/>
     </row>
-    <row r="1173" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1173" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1173" s="26"/>
       <c r="H1173" s="6"/>
     </row>
-    <row r="1174" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1174" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1174" s="26"/>
       <c r="H1174" s="6"/>
     </row>
-    <row r="1175" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1175" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1175" s="26"/>
       <c r="H1175" s="6"/>
     </row>
-    <row r="1176" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1176" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1176" s="26"/>
       <c r="H1176" s="6"/>
     </row>
-    <row r="1177" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1177" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1177" s="26"/>
       <c r="H1177" s="6"/>
     </row>
-    <row r="1178" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1178" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1178" s="26"/>
       <c r="H1178" s="6"/>
     </row>
-    <row r="1179" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1179" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1179" s="26"/>
       <c r="H1179" s="6"/>
     </row>
-    <row r="1180" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1180" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1180" s="26"/>
       <c r="H1180" s="6"/>
     </row>
-    <row r="1181" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1181" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1181" s="26"/>
       <c r="H1181" s="6"/>
     </row>
-    <row r="1182" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1182" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1182" s="26"/>
       <c r="H1182" s="6"/>
     </row>
-    <row r="1183" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1183" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1183" s="26"/>
       <c r="H1183" s="6"/>
     </row>
-    <row r="1184" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1184" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1184" s="26"/>
       <c r="H1184" s="6"/>
     </row>
-    <row r="1185" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1185" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1185" s="26"/>
       <c r="H1185" s="6"/>
     </row>
-    <row r="1186" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1186" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1186" s="26"/>
       <c r="H1186" s="6"/>
     </row>
-    <row r="1187" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1187" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1187" s="26"/>
       <c r="H1187" s="6"/>
     </row>
-    <row r="1188" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1188" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1188" s="26"/>
       <c r="H1188" s="27"/>
     </row>
-    <row r="1189" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1189" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1189" s="26"/>
       <c r="H1189" s="27"/>
     </row>
-    <row r="1190" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1190" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1190" s="26"/>
       <c r="H1190" s="27"/>
     </row>
-    <row r="1191" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1191" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1191" s="26"/>
       <c r="H1191" s="27"/>
     </row>
-    <row r="1192" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1192" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1192" s="26"/>
       <c r="H1192" s="27"/>
     </row>
-    <row r="1193" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1193" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1193" s="26"/>
       <c r="H1193" s="27"/>
     </row>
-    <row r="1194" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1194" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1194" s="26"/>
       <c r="H1194" s="27"/>
     </row>
-    <row r="1195" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1195" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1195" s="26"/>
       <c r="H1195" s="27"/>
     </row>
-    <row r="1196" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1196" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1196" s="26"/>
       <c r="H1196" s="27"/>
     </row>
-    <row r="1197" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1197" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1197" s="26"/>
       <c r="H1197" s="27"/>
     </row>
-    <row r="1198" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1198" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1198" s="26"/>
       <c r="H1198" s="27"/>
     </row>
-    <row r="1199" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1199" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1199" s="26"/>
       <c r="H1199" s="6"/>
     </row>
-    <row r="1200" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1200" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1200" s="26"/>
       <c r="H1200" s="6"/>
     </row>
-    <row r="1201" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1201" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1201" s="26"/>
       <c r="H1201" s="6"/>
     </row>
-    <row r="1202" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1202" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1202" s="26"/>
       <c r="H1202" s="6"/>
     </row>
-    <row r="1203" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1203" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1203" s="26"/>
       <c r="H1203" s="6"/>
     </row>
-    <row r="1204" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1204" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1204" s="26"/>
       <c r="H1204" s="6"/>
     </row>
-    <row r="1205" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1205" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1205" s="26"/>
       <c r="H1205" s="6"/>
     </row>
-    <row r="1206" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1206" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1206" s="26"/>
       <c r="H1206" s="6"/>
     </row>
-    <row r="1207" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1207" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1207" s="26"/>
       <c r="H1207" s="6"/>
     </row>
-    <row r="1208" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1208" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1208" s="26"/>
       <c r="H1208" s="6"/>
     </row>
-    <row r="1209" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1209" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1209" s="26"/>
       <c r="H1209" s="6"/>
     </row>
-    <row r="1210" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1210" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1210" s="26"/>
       <c r="H1210" s="6"/>
     </row>
-    <row r="1211" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1211" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1211" s="26"/>
       <c r="H1211" s="6"/>
     </row>
-    <row r="1212" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1212" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1212" s="26"/>
       <c r="H1212" s="6"/>
     </row>
-    <row r="1213" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1213" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1213" s="26"/>
       <c r="H1213" s="6"/>
     </row>
-    <row r="1214" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1214" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1214" s="26"/>
       <c r="H1214" s="6"/>
     </row>
-    <row r="1215" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1215" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1215" s="26"/>
       <c r="H1215" s="6"/>
     </row>
-    <row r="1216" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1216" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1216" s="26"/>
       <c r="H1216" s="6"/>
     </row>
-    <row r="1217" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1217" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1217" s="26"/>
       <c r="H1217" s="6"/>
     </row>
-    <row r="1218" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1218" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1218" s="26"/>
       <c r="H1218" s="6"/>
     </row>
-    <row r="1219" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1219" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1219" s="26"/>
       <c r="H1219" s="6"/>
     </row>
-    <row r="1220" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1220" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1220" s="26"/>
       <c r="H1220" s="29"/>
     </row>
-    <row r="1221" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1221" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1221" s="26"/>
       <c r="H1221" s="29"/>
     </row>
-    <row r="1222" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1222" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1222" s="26"/>
       <c r="H1222" s="29"/>
     </row>
-    <row r="1223" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1223" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1223" s="26"/>
       <c r="H1223" s="29"/>
     </row>
-    <row r="1224" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1224" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1224" s="26"/>
       <c r="H1224" s="29"/>
     </row>
-    <row r="1225" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1225" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1225" s="26"/>
       <c r="H1225" s="29"/>
     </row>
-    <row r="1226" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1226" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1226" s="26"/>
       <c r="H1226" s="29"/>
     </row>
-    <row r="1227" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1227" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1227" s="26"/>
       <c r="H1227" s="29"/>
     </row>
-    <row r="1228" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1228" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1228" s="26"/>
       <c r="H1228" s="29"/>
     </row>
-    <row r="1229" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1229" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1229" s="26"/>
       <c r="H1229" s="29"/>
     </row>
-    <row r="1230" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1230" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1230" s="26"/>
       <c r="H1230" s="29"/>
     </row>
-    <row r="1231" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1231" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1231" s="26"/>
       <c r="H1231" s="29"/>
     </row>
-    <row r="1232" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1232" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1232" s="26"/>
       <c r="H1232" s="29"/>
     </row>
-    <row r="1233" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1233" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1233" s="26"/>
       <c r="H1233" s="29"/>
     </row>
-    <row r="1234" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1234" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1234" s="26"/>
       <c r="H1234" s="29"/>
     </row>
-    <row r="1235" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1235" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1235" s="26"/>
       <c r="H1235" s="29"/>
     </row>
-    <row r="1236" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1236" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1236" s="26"/>
       <c r="H1236" s="29"/>
     </row>
-    <row r="1237" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1237" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1237" s="26"/>
       <c r="H1237" s="1"/>
     </row>
-    <row r="1238" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1238" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1238" s="26"/>
       <c r="H1238" s="1"/>
     </row>
-    <row r="1239" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1239" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1239" s="26"/>
       <c r="H1239" s="1"/>
     </row>
-    <row r="1240" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1240" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1240" s="26"/>
       <c r="H1240" s="1"/>
     </row>
-    <row r="1241" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1241" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1241" s="26"/>
       <c r="H1241" s="1"/>
     </row>
-    <row r="1242" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1242" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1242" s="26"/>
       <c r="H1242" s="1"/>
     </row>
-    <row r="1243" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1243" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1243" s="26"/>
       <c r="H1243" s="1"/>
     </row>
-    <row r="1244" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1244" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1244" s="26"/>
       <c r="H1244" s="1"/>
     </row>
-    <row r="1245" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1245" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1245" s="26"/>
       <c r="H1245" s="1"/>
     </row>
-    <row r="1246" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1246" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1246" s="26"/>
       <c r="H1246" s="1"/>
     </row>
-    <row r="1247" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1247" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1247" s="26"/>
       <c r="H1247" s="1"/>
     </row>
-    <row r="1248" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1248" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1248" s="26"/>
       <c r="H1248" s="1"/>
     </row>
-    <row r="1249" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1249" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1249" s="26"/>
       <c r="H1249" s="1"/>
     </row>
-    <row r="1250" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1250" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1250" s="26"/>
       <c r="H1250" s="1"/>
     </row>
-    <row r="1251" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1251" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1251" s="26"/>
       <c r="H1251" s="1"/>
     </row>
-    <row r="1252" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1252" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1252" s="26"/>
       <c r="H1252" s="1"/>
     </row>
-    <row r="1253" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1253" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1253" s="26"/>
       <c r="H1253" s="1"/>
     </row>
-    <row r="1254" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1254" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1254" s="26"/>
       <c r="H1254" s="1"/>
     </row>
-    <row r="1255" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1255" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1255" s="26"/>
       <c r="H1255" s="1"/>
     </row>
-    <row r="1256" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1256" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1256" s="26"/>
       <c r="H1256" s="1"/>
     </row>
-    <row r="1257" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1257" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1257" s="26"/>
       <c r="H1257" s="1"/>
     </row>
-    <row r="1258" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1258" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1258" s="26"/>
       <c r="H1258" s="1"/>
     </row>
-    <row r="1259" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1259" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1259" s="26"/>
       <c r="H1259" s="1"/>
     </row>
-    <row r="1260" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1260" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1260" s="26"/>
       <c r="H1260" s="1"/>
     </row>
-    <row r="1261" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1261" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1261" s="26"/>
       <c r="H1261" s="1"/>
     </row>
-    <row r="1262" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1262" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1262" s="26"/>
       <c r="H1262" s="1"/>
     </row>
-    <row r="1263" spans="7:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1263" spans="7:8" ht="16" x14ac:dyDescent="0.2">
       <c r="G1263" s="26"/>
       <c r="H1263" s="1"/>
     </row>
@@ -4657,12 +4660,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -4670,7 +4673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -4678,7 +4681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="8"/>
       <c r="C3" s="6"/>
@@ -4727,7 +4730,7 @@
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
     </row>
-    <row r="4" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="9"/>
       <c r="C4" s="4"/>
@@ -4776,155 +4779,155 @@
       <c r="AT4" s="4"/>
       <c r="AU4" s="4"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
     </row>
   </sheetData>
@@ -4934,6 +4937,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A396E11C201049A295728E554B4204" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5308e23870a69a858a1f647203e717c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e" xmlns:ns3="61093040-1240-489f-8ca6-d5903aeb7a38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f096f016f089f4e04afada0be9633fb" ns2:_="" ns3:_="">
     <xsd:import namespace="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
@@ -5130,36 +5148,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3E4B6-7659-40E5-A3BE-8806173B61A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
-    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5182,9 +5174,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3E4B6-7659-40E5-A3BE-8806173B61A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
+    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added 100 to ID Hell's Canyon dataset numbers
</commit_message>
<xml_diff>
--- a/data/USFWS_bull_trout_SSA_data_ID_HellsCanyon.xlsx
+++ b/data/USFWS_bull_trout_SSA_data_ID_HellsCanyon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scheuerl/Documents/GitHub/bulltrout/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8404F2-985D-0246-AFF9-A11876E6CCAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A46892F-B7A3-1348-A35B-802FC775693B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:BB1263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -698,7 +698,7 @@
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>18</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>18</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>18</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>18</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>18</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>18</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>18</v>
@@ -1006,7 +1006,7 @@
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>18</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>18</v>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>18</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>18</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>18</v>
@@ -1196,7 +1196,7 @@
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>18</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>18</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>18</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>18</v>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>18</v>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>18</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>18</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>18</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="15">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>18</v>
@@ -4937,21 +4937,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056A396E11C201049A295728E554B4204" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5308e23870a69a858a1f647203e717c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e" xmlns:ns3="61093040-1240-489f-8ca6-d5903aeb7a38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6f096f016f089f4e04afada0be9633fb" ns2:_="" ns3:_="">
     <xsd:import namespace="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
@@ -5148,10 +5133,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3E4B6-7659-40E5-A3BE-8806173B61A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
+    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5174,20 +5185,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29F3E4B6-7659-40E5-A3BE-8806173B61A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFAABD42-B977-47B6-983A-D015976BBDFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="dbfd3e1b-9f3f-4f6f-b75c-e8eed26c7c7e"/>
-    <ds:schemaRef ds:uri="61093040-1240-489f-8ca6-d5903aeb7a38"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>